<commit_message>
index test case updated with real data.
</commit_message>
<xml_diff>
--- a/Tests/Test Cases/index.xlsx
+++ b/Tests/Test Cases/index.xlsx
@@ -5,11 +5,11 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tthakgunduz/Desktop/SWE574/GiTHUB/docs-repo/Tests/Test Cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tthakgunduz/Desktop/ALL/Master-BOUN/SWE574/GiTHUB/docs-repo/Tests/Test Cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="3920" windowWidth="24000" windowHeight="13560"/>
+    <workbookView xWindow="420" yWindow="5480" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Task Name</t>
   </si>
@@ -62,9 +62,6 @@
     <t>User opens http://localhost:8080/index.html page.</t>
   </si>
   <si>
-    <t>If there are 4 or more communities, 4 communities are listed with See More option. If not, all communities are listed.</t>
-  </si>
-  <si>
     <t>1- Open main page.
 2- Click on See More button</t>
   </si>
@@ -78,14 +75,6 @@
     <t>User searches community.</t>
   </si>
   <si>
-    <t>Community section is updated with results.</t>
-  </si>
-  <si>
-    <t>1- Open main page.
-2- Enter keyword in search field.
-3- Press enter or click on search button</t>
-  </si>
-  <si>
     <t>#99</t>
   </si>
   <si>
@@ -125,10 +114,6 @@
     <t>User displays the communities having a popular group tag.</t>
   </si>
   <si>
-    <t>1- Open main page.
-2- Click on a popular group tag.</t>
-  </si>
-  <si>
     <t>#172</t>
   </si>
   <si>
@@ -151,18 +136,36 @@
     <t>Please log in to join community dialog shows up.</t>
   </si>
   <si>
+    <t>User views community details.</t>
+  </si>
+  <si>
+    <t>Community details page is opened.</t>
+  </si>
+  <si>
+    <t>Communities are listed.</t>
+  </si>
+  <si>
     <t>1- Open main page.
-2- Click on join button on one of community.</t>
-  </si>
-  <si>
-    <t>User views community details.</t>
+2- Enter web keyword in search field.
+3- Press enter or click on search button</t>
+  </si>
+  <si>
+    <t>Community section is updated with results having web keyword in it.</t>
   </si>
   <si>
     <t>1- Open main page.
-2- Click on community details button on one of community.</t>
-  </si>
-  <si>
-    <t>Community details page is opened.</t>
+2- Click on "web" popular group tag.</t>
+  </si>
+  <si>
+    <t>Community section is updated with results having web tag in it.</t>
+  </si>
+  <si>
+    <t>1- Open main page.
+2- Click on join button on "Web Community" community.</t>
+  </si>
+  <si>
+    <t>1- Open main page.
+2- Click on community details button on "Web Community".</t>
   </si>
 </sst>
 </file>
@@ -342,6 +345,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -350,9 +356,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -670,16 +673,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -691,10 +694,10 @@
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -703,7 +706,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -711,7 +714,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>9</v>
@@ -728,13 +731,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
@@ -746,17 +749,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -766,13 +769,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
@@ -784,13 +787,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
@@ -802,17 +805,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -822,17 +825,17 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -842,17 +845,17 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -862,13 +865,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="9"/>
@@ -880,13 +883,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="9"/>

</xml_diff>